<commit_message>
# Marcar uma classe como um bean.- Spring Boot
</commit_message>
<xml_diff>
--- a/plano_de_estudo_micronaut.xlsx
+++ b/plano_de_estudo_micronaut.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Exploração prévia (opcional)" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>Fonte</t>
   </si>
@@ -225,6 +225,12 @@
     <t>https://guides.micronaut.io/latest/building-a-rest-api-spring-boot-vs-micronaut-security-basic-auth.html</t>
   </si>
   <si>
+    <t>https://guides.micronaut.io/latest/spring-boot-to-micronaut-application-class-maven-java.html</t>
+  </si>
+  <si>
+    <t>https://guides.micronaut.io/latest/spring-boot-to-micronaut-at-singleton-at-component-maven-java.html</t>
+  </si>
+  <si>
     <t>Exercício</t>
   </si>
   <si>
@@ -309,7 +315,7 @@
   <fonts count="5">
     <font>
       <sz val="10.000000"/>
-      <color indexed="64"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -356,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -371,9 +377,7 @@
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11973,7 +11977,7 @@
       <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -11988,7 +11992,7 @@
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -23114,24 +23118,24 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-      <c r="AC2" s="8"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
     </row>
     <row r="3" ht="63.75">
       <c r="A3" s="1"/>
@@ -23145,24 +23149,24 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="8"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
     </row>
     <row r="4" ht="25.5">
       <c r="A4" s="3" t="s">
@@ -23175,8 +23179,12 @@
       <c r="D4" s="4">
         <v>4</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="E4" s="4">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -23194,8 +23202,12 @@
       <c r="D5" s="4">
         <v>4</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="E5" s="4">
+        <v>5</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -23935,8 +23947,12 @@
       <c r="D44" s="4">
         <v>4</v>
       </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
+      <c r="E44" s="4">
+        <v>5</v>
+      </c>
+      <c r="F44" s="4">
+        <v>1</v>
+      </c>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
@@ -23944,12 +23960,22 @@
       <c r="K44" s="4"/>
     </row>
     <row r="45">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
+      <c r="A45" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="4">
+        <v>4</v>
+      </c>
       <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
+      <c r="D45" s="4">
+        <v>4</v>
+      </c>
+      <c r="E45" s="4">
+        <v>5</v>
+      </c>
+      <c r="F45" s="4">
+        <v>1</v>
+      </c>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
@@ -23957,12 +23983,22 @@
       <c r="K45" s="4"/>
     </row>
     <row r="46">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
+      <c r="A46" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="4">
+        <v>4</v>
+      </c>
       <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
+      <c r="D46" s="4">
+        <v>4</v>
+      </c>
+      <c r="E46" s="4">
+        <v>5</v>
+      </c>
+      <c r="F46" s="4">
+        <v>1</v>
+      </c>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
@@ -36401,6 +36437,8 @@
     <hyperlink r:id="rId39" ref="A42"/>
     <hyperlink r:id="rId38" ref="A43"/>
     <hyperlink r:id="rId39" ref="A44"/>
+    <hyperlink r:id="rId40" ref="A45"/>
+    <hyperlink r:id="rId41" ref="A46"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -36429,25 +36467,25 @@
   <sheetData>
     <row r="1" ht="63.75">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -36484,7 +36522,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B3" s="4">
         <v>4</v>
@@ -36497,7 +36535,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B4" s="4">
         <v>4</v>
@@ -36510,7 +36548,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
@@ -36523,7 +36561,7 @@
     </row>
     <row r="6" ht="25.5">
       <c r="A6" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B6" s="4">
         <v>4</v>
@@ -36536,7 +36574,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B7" s="4">
         <v>4</v>
@@ -36549,7 +36587,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B8" s="4">
         <v>4</v>
@@ -36562,7 +36600,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B9" s="4">
         <v>4</v>
@@ -36575,7 +36613,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B10" s="4">
         <v>4</v>
@@ -36588,7 +36626,7 @@
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B11" s="4">
         <v>4</v>
@@ -36601,7 +36639,7 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B12" s="4">
         <v>4</v>
@@ -36614,7 +36652,7 @@
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B13" s="4">
         <v>4</v>
@@ -36627,7 +36665,7 @@
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B14" s="4">
         <v>4</v>
@@ -36640,7 +36678,7 @@
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B15" s="4">
         <v>4</v>
@@ -36653,7 +36691,7 @@
     </row>
     <row r="16" ht="25.5">
       <c r="A16" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B16" s="4">
         <v>4</v>
@@ -45563,23 +45601,23 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>89</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
     <row r="3">
-      <c r="A3" s="7" t="s">
-        <v>90</v>
+      <c r="A3" s="6" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="4">
@@ -48569,7 +48607,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{000500EA-0018-4587-B1CB-00CA00F10065}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00A000A1-0057-449B-9232-00E300D30029}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
           <x14:formula1>
             <xm:f>"Feeling sobre o quão confortável está com aquilo,Usa a llm pedindo feedback (óbvio que a llm pode errar),Comparação do que você fez com de outra pessoa com um nível de senioridade maior,Postagem do que você fez em redes públicas para tentar pegar feedback"&amp;".  ,Feedbacks de pares do trabalho sobre determinado fase do plano, entregável, entendimento etc,Acesso a uma pessoa professora que pode te dar feedback direto"</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
#Testando serialização spring boot vs micronaut - criando rest api
</commit_message>
<xml_diff>
--- a/plano_de_estudo_micronaut.xlsx
+++ b/plano_de_estudo_micronaut.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>Fonte</t>
   </si>
@@ -234,6 +234,12 @@
     <t>https://guides.micronaut.io/latest/spring-boot-to-micronaut-uri-components-builder-vs-uri-builder-maven-java.html</t>
   </si>
   <si>
+    <t>https://guides.micronaut.io/latest/micronaut-spring-boot-maven-java.html</t>
+  </si>
+  <si>
+    <t>https://guides.micronaut.io/latest/spring-boot-micronaut-data-gradle-java.html</t>
+  </si>
+  <si>
     <t>Exercício</t>
   </si>
   <si>
@@ -315,9 +321,21 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10.000000"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -345,15 +363,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+        <bgColor indexed="26"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -361,29 +391,54 @@
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="2" fillId="3" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="0" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="1" fillId="3" borderId="1" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -23807,38 +23862,42 @@
       <c r="K36" s="4"/>
     </row>
     <row r="37">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="7">
         <v>4</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4">
+      <c r="C37" s="7"/>
+      <c r="D37" s="7">
         <v>4</v>
       </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="E37" s="7">
+        <v>5</v>
+      </c>
+      <c r="F37" s="7">
+        <v>1</v>
+      </c>
+      <c r="G37" s="7"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
     </row>
     <row r="38">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="7">
         <v>4</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4">
+      <c r="C38" s="7"/>
+      <c r="D38" s="7">
         <v>4</v>
       </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
@@ -23940,118 +23999,138 @@
       <c r="K43" s="4"/>
     </row>
     <row r="44">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B44" s="7">
         <v>4</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4">
+      <c r="C44" s="7"/>
+      <c r="D44" s="7">
         <v>4</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="7">
         <v>5</v>
       </c>
-      <c r="F44" s="4">
+      <c r="F44" s="7">
         <v>1</v>
       </c>
-      <c r="G44" s="4"/>
+      <c r="G44" s="7"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
     </row>
     <row r="45">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B45" s="7">
         <v>4</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4">
+      <c r="C45" s="7"/>
+      <c r="D45" s="7">
         <v>4</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="7">
         <v>5</v>
       </c>
-      <c r="F45" s="4">
+      <c r="F45" s="7">
         <v>1</v>
       </c>
-      <c r="G45" s="4"/>
+      <c r="G45" s="7"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
     </row>
     <row r="46">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" s="7">
         <v>4</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4">
+      <c r="C46" s="7"/>
+      <c r="D46" s="7">
         <v>4</v>
       </c>
-      <c r="E46" s="4">
+      <c r="E46" s="7">
         <v>5</v>
       </c>
-      <c r="F46" s="4">
+      <c r="F46" s="7">
         <v>1</v>
       </c>
-      <c r="G46" s="4"/>
+      <c r="G46" s="7"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
     </row>
     <row r="47">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B47" s="4">
+      <c r="B47" s="7">
         <v>4</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4">
+      <c r="C47" s="7"/>
+      <c r="D47" s="7">
         <v>4</v>
       </c>
-      <c r="E47" s="4">
+      <c r="E47" s="7">
         <v>5</v>
       </c>
-      <c r="F47" s="4">
+      <c r="F47" s="7">
         <v>1</v>
       </c>
-      <c r="G47" s="4"/>
+      <c r="G47" s="7"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
     </row>
     <row r="48">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
+      <c r="A48" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" s="8">
+        <v>4</v>
+      </c>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8">
+        <v>4</v>
+      </c>
+      <c r="E48" s="8">
+        <v>5</v>
+      </c>
+      <c r="F48" s="8">
+        <v>1</v>
+      </c>
+      <c r="G48" s="8"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
     </row>
     <row r="49">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
+      <c r="A49" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" s="8">
+        <v>4</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8">
+        <v>4</v>
+      </c>
+      <c r="E49" s="8">
+        <v>5</v>
+      </c>
+      <c r="F49" s="8">
+        <v>1</v>
+      </c>
+      <c r="G49" s="8"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
@@ -36453,6 +36532,8 @@
     <hyperlink r:id="rId40" ref="A45"/>
     <hyperlink r:id="rId41" ref="A46"/>
     <hyperlink r:id="rId42" ref="A47"/>
+    <hyperlink r:id="rId43" ref="A48"/>
+    <hyperlink r:id="rId44" ref="A49"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -36481,25 +36562,25 @@
   <sheetData>
     <row r="1" ht="63.75">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -36536,7 +36617,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B3" s="4">
         <v>4</v>
@@ -36549,7 +36630,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B4" s="4">
         <v>4</v>
@@ -36562,7 +36643,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
@@ -36575,7 +36656,7 @@
     </row>
     <row r="6" ht="25.5">
       <c r="A6" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B6" s="4">
         <v>4</v>
@@ -36588,7 +36669,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B7" s="4">
         <v>4</v>
@@ -36601,7 +36682,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B8" s="4">
         <v>4</v>
@@ -36614,7 +36695,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B9" s="4">
         <v>4</v>
@@ -36627,7 +36708,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B10" s="4">
         <v>4</v>
@@ -36640,7 +36721,7 @@
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B11" s="4">
         <v>4</v>
@@ -36653,7 +36734,7 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B12" s="4">
         <v>4</v>
@@ -36666,7 +36747,7 @@
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B13" s="4">
         <v>4</v>
@@ -36679,7 +36760,7 @@
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B14" s="4">
         <v>4</v>
@@ -36692,7 +36773,7 @@
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B15" s="4">
         <v>4</v>
@@ -36705,7 +36786,7 @@
     </row>
     <row r="16" ht="25.5">
       <c r="A16" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B16" s="4">
         <v>4</v>
@@ -45615,23 +45696,23 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4">
@@ -48621,7 +48702,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0007008D-00A9-43C1-BF06-00C8009D00BE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00E9008B-0060-429E-97E1-00CB00BD00B6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
           <x14:formula1>
             <xm:f>"Feeling sobre o quão confortável está com aquilo,Usa a llm pedindo feedback (óbvio que a llm pode errar),Comparação do que você fez com de outra pessoa com um nível de senioridade maior,Postagem do que você fez em redes públicas para tentar pegar feedback"&amp;".  ,Feedbacks de pares do trabalho sobre determinado fase do plano, entregável, entendimento etc,Acesso a uma pessoa professora que pode te dar feedback direto"</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Micronaut Dependency Injection Types
</commit_message>
<xml_diff>
--- a/plano_de_estudo_micronaut.xlsx
+++ b/plano_de_estudo_micronaut.xlsx
@@ -23227,84 +23227,92 @@
       <c r="AC3" s="2"/>
     </row>
     <row r="4" ht="25.5">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="7">
         <v>4</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7">
         <v>4</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="7">
         <v>5</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="7">
         <v>1</v>
       </c>
-      <c r="G4" s="4"/>
+      <c r="G4" s="7"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" ht="38.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="7">
         <v>4</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7">
         <v>4</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="7">
         <v>5</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="7">
         <v>1</v>
       </c>
-      <c r="G5" s="4"/>
+      <c r="G5" s="7"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
     <row r="6" ht="38.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="7">
         <v>4</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7">
         <v>4</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="E6" s="7">
+        <v>5</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
     <row r="7" ht="38.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="7">
         <v>4</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7">
         <v>4</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="E7" s="7">
+        <v>5</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="7"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -23904,101 +23912,121 @@
       <c r="K38" s="4"/>
     </row>
     <row r="39">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="7">
         <v>4</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4">
+      <c r="C39" s="7"/>
+      <c r="D39" s="7">
         <v>4</v>
       </c>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
+      <c r="E39" s="7">
+        <v>5</v>
+      </c>
+      <c r="F39" s="7">
+        <v>1</v>
+      </c>
+      <c r="G39" s="7"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
     </row>
     <row r="40">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="7">
         <v>4</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4">
+      <c r="C40" s="7"/>
+      <c r="D40" s="7">
         <v>4</v>
       </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="E40" s="7">
+        <v>5</v>
+      </c>
+      <c r="F40" s="7">
+        <v>1</v>
+      </c>
+      <c r="G40" s="7"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
     </row>
     <row r="41">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="7">
         <v>4</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4">
+      <c r="C41" s="7"/>
+      <c r="D41" s="7">
         <v>4</v>
       </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
+      <c r="E41" s="7">
+        <v>5</v>
+      </c>
+      <c r="F41" s="7">
+        <v>1</v>
+      </c>
+      <c r="G41" s="7"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
     </row>
-    <row r="42">
-      <c r="A42" s="3" t="s">
+    <row r="42" ht="28.5">
+      <c r="A42" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="7">
         <v>4</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4">
+      <c r="C42" s="7"/>
+      <c r="D42" s="7">
         <v>4</v>
       </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
+      <c r="E42" s="7">
+        <v>5</v>
+      </c>
+      <c r="F42" s="7">
+        <v>1</v>
+      </c>
+      <c r="G42" s="7"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
     </row>
     <row r="43">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" s="7">
         <v>4</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4">
+      <c r="C43" s="7"/>
+      <c r="D43" s="7">
         <v>4</v>
       </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
+      <c r="E43" s="7">
+        <v>5</v>
+      </c>
+      <c r="F43" s="7">
+        <v>1</v>
+      </c>
+      <c r="G43" s="7"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
     </row>
-    <row r="44">
+    <row r="44" ht="28.5">
       <c r="A44" s="7" t="s">
         <v>65</v>
       </c>
@@ -24044,7 +24072,7 @@
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
     </row>
-    <row r="46">
+    <row r="46" ht="28.5">
       <c r="A46" s="7" t="s">
         <v>67</v>
       </c>
@@ -24067,7 +24095,7 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
     </row>
-    <row r="47">
+    <row r="47" ht="28.5">
       <c r="A47" s="7" t="s">
         <v>68</v>
       </c>
@@ -48702,7 +48730,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00E9008B-0060-429E-97E1-00CB00BD00B6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+        <x14:dataValidation xr:uid="{000200C7-0056-41D7-9F19-0072002A00F9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
           <x14:formula1>
             <xm:f>"Feeling sobre o quão confortável está com aquilo,Usa a llm pedindo feedback (óbvio que a llm pode errar),Comparação do que você fez com de outra pessoa com um nível de senioridade maior,Postagem do que você fez em redes públicas para tentar pegar feedback"&amp;".  ,Feedbacks de pares do trabalho sobre determinado fase do plano, entregável, entendimento etc,Acesso a uma pessoa professora que pode te dar feedback direto"</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Tipos de escopo Micronaut
</commit_message>
<xml_diff>
--- a/plano_de_estudo_micronaut.xlsx
+++ b/plano_de_estudo_micronaut.xlsx
@@ -23319,19 +23319,23 @@
       <c r="K7" s="4"/>
     </row>
     <row r="8" ht="38.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="7">
         <v>4</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7">
         <v>4</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="E8" s="7">
+        <v>5</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
+      </c>
+      <c r="G8" s="7"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -48730,7 +48734,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{000200C7-0056-41D7-9F19-0072002A00F9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00830097-0046-4ED4-8A69-00FE00410034}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
           <x14:formula1>
             <xm:f>"Feeling sobre o quão confortável está com aquilo,Usa a llm pedindo feedback (óbvio que a llm pode errar),Comparação do que você fez com de outra pessoa com um nível de senioridade maior,Postagem do que você fez em redes públicas para tentar pegar feedback"&amp;".  ,Feedbacks de pares do trabalho sobre determinado fase do plano, entregável, entendimento etc,Acesso a uma pessoa professora que pode te dar feedback direto"</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Testando integrações de API REST usando Testcontainers com WireMock ou MockServer
</commit_message>
<xml_diff>
--- a/plano_de_estudo_micronaut.xlsx
+++ b/plano_de_estudo_micronaut.xlsx
@@ -23460,19 +23460,23 @@
       <c r="K13" s="4"/>
     </row>
     <row r="14" ht="51">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="7">
         <v>4</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4">
+      <c r="C14" s="7"/>
+      <c r="D14" s="7">
         <v>4</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="E14" s="7">
+        <v>5</v>
+      </c>
+      <c r="F14" s="7">
+        <v>1</v>
+      </c>
+      <c r="G14" s="7"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -48777,7 +48781,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00110037-00F9-40BC-895B-0011007000EA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00530022-000F-47E7-9409-0072008F008C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
           <x14:formula1>
             <xm:f>"Feeling sobre o quão confortável está com aquilo,Usa a llm pedindo feedback (óbvio que a llm pode errar),Comparação do que você fez com de outra pessoa com um nível de senioridade maior,Postagem do que você fez em redes públicas para tentar pegar feedback"&amp;".  ,Feedbacks de pares do trabalho sobre determinado fase do plano, entregável, entendimento etc,Acesso a uma pessoa professora que pode te dar feedback direto"</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Micronaut Data and Java Records
</commit_message>
<xml_diff>
--- a/plano_de_estudo_micronaut.xlsx
+++ b/plano_de_estudo_micronaut.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>Fonte</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>https://guides.micronaut.io/latest/micronaut-cache.html</t>
+  </si>
+  <si>
+    <t>https://guides.micronaut.io/latest/micronaut-java-records-maven-java.html</t>
   </si>
   <si>
     <t>https://guides.micronaut.io/latest/micronaut-patterns-composite.html</t>
@@ -23522,7 +23525,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" ht="38.25">
+    <row r="17" ht="25.5">
       <c r="A17" s="7" t="s">
         <v>40</v>
       </c>
@@ -23546,19 +23549,23 @@
       <c r="K17" s="4"/>
     </row>
     <row r="18" ht="38.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="7">
         <v>4</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4">
+      <c r="C18" s="7"/>
+      <c r="D18" s="7">
         <v>4</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="E18" s="7">
+        <v>5</v>
+      </c>
+      <c r="F18" s="7">
+        <v>1</v>
+      </c>
+      <c r="G18" s="7"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -23678,7 +23685,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" ht="25.5">
+    <row r="25" ht="38.25">
       <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
@@ -23697,7 +23704,7 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" ht="38.25">
+    <row r="26" ht="25.5">
       <c r="A26" s="3" t="s">
         <v>49</v>
       </c>
@@ -23792,24 +23799,20 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
     </row>
-    <row r="31">
-      <c r="A31" s="7" t="s">
+    <row r="31" ht="38.25">
+      <c r="A31" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="4">
         <v>4</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7">
+      <c r="C31" s="4"/>
+      <c r="D31" s="4">
         <v>4</v>
       </c>
-      <c r="E31" s="7">
-        <v>5</v>
-      </c>
-      <c r="F31" s="7">
-        <v>1</v>
-      </c>
-      <c r="G31" s="7"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
@@ -23839,19 +23842,23 @@
       <c r="K32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="7">
         <v>4</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4">
+      <c r="C33" s="7"/>
+      <c r="D33" s="7">
         <v>4</v>
       </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="E33" s="7">
+        <v>5</v>
+      </c>
+      <c r="F33" s="7">
+        <v>1</v>
+      </c>
+      <c r="G33" s="7"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
@@ -23896,23 +23903,19 @@
       <c r="K35" s="4"/>
     </row>
     <row r="36">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="4">
         <v>4</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7">
+      <c r="C36" s="4"/>
+      <c r="D36" s="4">
         <v>4</v>
       </c>
-      <c r="E36" s="7">
-        <v>5</v>
-      </c>
-      <c r="F36" s="7">
-        <v>1</v>
-      </c>
-      <c r="G36" s="7"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
@@ -23929,8 +23932,12 @@
       <c r="D37" s="7">
         <v>4</v>
       </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="E37" s="7">
+        <v>5</v>
+      </c>
+      <c r="F37" s="7">
+        <v>1</v>
+      </c>
       <c r="G37" s="7"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
@@ -23948,12 +23955,8 @@
       <c r="D38" s="7">
         <v>4</v>
       </c>
-      <c r="E38" s="7">
-        <v>5</v>
-      </c>
-      <c r="F38" s="7">
-        <v>1</v>
-      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
       <c r="G38" s="7"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
@@ -24006,7 +24009,7 @@
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
     </row>
-    <row r="41" ht="28.5">
+    <row r="41">
       <c r="A41" s="7" t="s">
         <v>64</v>
       </c>
@@ -24029,9 +24032,9 @@
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
     </row>
-    <row r="42">
+    <row r="42" ht="28.5">
       <c r="A42" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B42" s="7">
         <v>4</v>
@@ -24052,7 +24055,7 @@
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" ht="28.5">
+    <row r="43">
       <c r="A43" s="7" t="s">
         <v>64</v>
       </c>
@@ -24075,7 +24078,7 @@
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
     </row>
-    <row r="44">
+    <row r="44" ht="28.5">
       <c r="A44" s="7" t="s">
         <v>65</v>
       </c>
@@ -24098,7 +24101,7 @@
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
     </row>
-    <row r="45" ht="28.5">
+    <row r="45">
       <c r="A45" s="7" t="s">
         <v>66</v>
       </c>
@@ -24144,24 +24147,24 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
     </row>
-    <row r="47">
-      <c r="A47" s="8" t="s">
+    <row r="47" ht="28.5">
+      <c r="A47" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="7">
         <v>4</v>
       </c>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8">
+      <c r="C47" s="7"/>
+      <c r="D47" s="7">
         <v>4</v>
       </c>
-      <c r="E47" s="8">
+      <c r="E47" s="7">
         <v>5</v>
       </c>
-      <c r="F47" s="8">
+      <c r="F47" s="7">
         <v>1</v>
       </c>
-      <c r="G47" s="8"/>
+      <c r="G47" s="7"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
@@ -24191,13 +24194,23 @@
       <c r="K48" s="4"/>
     </row>
     <row r="49">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
+      <c r="A49" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" s="8">
+        <v>4</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8">
+        <v>4</v>
+      </c>
+      <c r="E49" s="8">
+        <v>5</v>
+      </c>
+      <c r="F49" s="8">
+        <v>1</v>
+      </c>
+      <c r="G49" s="8"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
@@ -36539,6 +36552,19 @@
       <c r="I998" s="4"/>
       <c r="J998" s="4"/>
       <c r="K998" s="4"/>
+    </row>
+    <row r="999">
+      <c r="A999" s="4"/>
+      <c r="B999" s="4"/>
+      <c r="C999" s="4"/>
+      <c r="D999" s="4"/>
+      <c r="E999" s="4"/>
+      <c r="F999" s="4"/>
+      <c r="G999" s="4"/>
+      <c r="H999" s="4"/>
+      <c r="I999" s="4"/>
+      <c r="J999" s="4"/>
+      <c r="K999" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -36580,13 +36606,14 @@
     <hyperlink r:id="rId36" ref="A39"/>
     <hyperlink r:id="rId37" ref="A40"/>
     <hyperlink r:id="rId38" ref="A41"/>
-    <hyperlink r:id="rId37" ref="A42"/>
+    <hyperlink r:id="rId39" ref="A42"/>
     <hyperlink r:id="rId38" ref="A43"/>
     <hyperlink r:id="rId39" ref="A44"/>
     <hyperlink r:id="rId40" ref="A45"/>
     <hyperlink r:id="rId41" ref="A46"/>
     <hyperlink r:id="rId42" ref="A47"/>
     <hyperlink r:id="rId43" ref="A48"/>
+    <hyperlink r:id="rId44" ref="A49"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -36615,25 +36642,25 @@
   <sheetData>
     <row r="1" ht="63.75">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -36670,7 +36697,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B3" s="4">
         <v>4</v>
@@ -36683,7 +36710,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B4" s="4">
         <v>4</v>
@@ -36696,7 +36723,7 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
@@ -36709,7 +36736,7 @@
     </row>
     <row r="6" ht="25.5">
       <c r="A6" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B6" s="4">
         <v>4</v>
@@ -36722,7 +36749,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B7" s="4">
         <v>4</v>
@@ -36735,7 +36762,7 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B8" s="4">
         <v>4</v>
@@ -36748,7 +36775,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B9" s="4">
         <v>4</v>
@@ -36761,7 +36788,7 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B10" s="4">
         <v>4</v>
@@ -36774,7 +36801,7 @@
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B11" s="4">
         <v>4</v>
@@ -36787,7 +36814,7 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B12" s="4">
         <v>4</v>
@@ -36800,7 +36827,7 @@
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B13" s="4">
         <v>4</v>
@@ -36813,7 +36840,7 @@
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B14" s="4">
         <v>4</v>
@@ -36826,7 +36853,7 @@
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B15" s="4">
         <v>4</v>
@@ -36839,7 +36866,7 @@
     </row>
     <row r="16" ht="25.5">
       <c r="A16" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B16" s="4">
         <v>4</v>
@@ -45749,23 +45776,23 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4">
@@ -48755,7 +48782,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{003300D4-0048-4D2A-B425-00AA008E00D2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+        <x14:dataValidation xr:uid="{009A00DA-0006-4E35-AF11-008200DC00CE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
           <x14:formula1>
             <xm:f>"Feeling sobre o quão confortável está com aquilo,Usa a llm pedindo feedback (óbvio que a llm pode errar),Comparação do que você fez com de outra pessoa com um nível de senioridade maior,Postagem do que você fez em redes públicas para tentar pegar feedback"&amp;".  ,Feedbacks de pares do trabalho sobre determinado fase do plano, entregável, entendimento etc,Acesso a uma pessoa professora que pode te dar feedback direto"</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
# Jpa e hibernate
</commit_message>
<xml_diff>
--- a/plano_de_estudo_micronaut.xlsx
+++ b/plano_de_estudo_micronaut.xlsx
@@ -23572,19 +23572,19 @@
       <c r="K18" s="4"/>
     </row>
     <row r="19" ht="38.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="7">
         <v>4</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4">
+      <c r="C19" s="7"/>
+      <c r="D19" s="7">
         <v>4</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -23648,19 +23648,23 @@
       <c r="K22" s="4"/>
     </row>
     <row r="23" ht="38.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="7">
         <v>4</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7">
         <v>4</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="E23" s="7">
+        <v>5</v>
+      </c>
+      <c r="F23" s="7">
+        <v>1</v>
+      </c>
+      <c r="G23" s="7"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -48782,7 +48786,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{009A00DA-0006-4E35-AF11-008200DC00CE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+        <x14:dataValidation xr:uid="{005A00D1-00F0-4E52-8B4C-001B00C80035}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
           <x14:formula1>
             <xm:f>"Feeling sobre o quão confortável está com aquilo,Usa a llm pedindo feedback (óbvio que a llm pode errar),Comparação do que você fez com de outra pessoa com um nível de senioridade maior,Postagem do que você fez em redes públicas para tentar pegar feedback"&amp;".  ,Feedbacks de pares do trabalho sobre determinado fase do plano, entregável, entendimento etc,Acesso a uma pessoa professora que pode te dar feedback direto"</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Autenticação básica do Micronaut
</commit_message>
<xml_diff>
--- a/plano_de_estudo_micronaut.xlsx
+++ b/plano_de_estudo_micronaut.xlsx
@@ -6,18 +6,49 @@
     <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Exploração prévia (opcional)" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Objetivo aprendizagem" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Alinhamento de expectativas" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Matriz de consumo de teorias" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Práticas prioritárias" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Mecanismos de feedback" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Exploração prévia (opcional)" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Objetivo aprendizagem" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Alinhamento de expectativas" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Matriz de consumo de teorias" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Práticas prioritárias" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Mecanismos de feedback" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={A12F5487-BD0A-1D55-ECB3-5B2E3E52411C}</author>
+  </authors>
+  <commentList>
+    <comment ref="G51" authorId="0" xr:uid="{A12F5487-BD0A-1D55-ECB3-5B2E3E52411C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>fsm:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+é necessari conhecimento sobre a api de reatividade do java, para entender os conceitos avançados de r2dbc
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -488,6 +519,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="fsm" id="{6C2C4E23-1051-674B-76A8-26210B26CEAD}" userId="fsm" providerId="Teamlab"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
@@ -980,6 +1017,15 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G51" dT="2025-05-08T15:38:14.08Z" personId="{6C2C4E23-1051-674B-76A8-26210B26CEAD}" id="{A12F5487-BD0A-1D55-ECB3-5B2E3E52411C}" done="0">
+    <text xml:space="preserve">é necessari conhecimento sobre a api de reatividade do java, para entender os conceitos avançados de r2dbc
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
@@ -23810,19 +23856,23 @@
       <c r="K28" s="4"/>
     </row>
     <row r="29" ht="38.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="7">
         <v>4</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4">
+      <c r="C29" s="7"/>
+      <c r="D29" s="7">
         <v>4</v>
       </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="E29" s="7">
+        <v>5</v>
+      </c>
+      <c r="F29" s="7">
+        <v>1</v>
+      </c>
+      <c r="G29" s="7"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -36681,6 +36731,7 @@
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
+  <legacyDrawing r:id="rId49"/>
 </worksheet>
 </file>
 
@@ -48844,7 +48895,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00CA00B7-00FC-4053-A68E-002C009D00DE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00CC0015-0089-4E6A-9C75-00F400FC0007}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
           <x14:formula1>
             <xm:f>"Feeling sobre o quão confortável está com aquilo,Usa a llm pedindo feedback (óbvio que a llm pode errar),Comparação do que você fez com de outra pessoa com um nível de senioridade maior,Postagem do que você fez em redes públicas para tentar pegar feedback"&amp;".  ,Feedbacks de pares do trabalho sobre determinado fase do plano, entregável, entendimento etc,Acesso a uma pessoa professora que pode te dar feedback direto"</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Content negotiation in a Micronaut Application
</commit_message>
<xml_diff>
--- a/plano_de_estudo_micronaut.xlsx
+++ b/plano_de_estudo_micronaut.xlsx
@@ -523,7 +523,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="fsm" id="{13C37F2E-4D51-E3EE-FC14-919C7A23FB02}" userId="fsm" providerId="Teamlab"/>
+  <person displayName="fsm" id="{97EA6DEE-8592-7F06-E67E-CB747DF27A81}" userId="fsm" providerId="Teamlab"/>
 </personList>
 </file>
 
@@ -1019,7 +1019,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G51" dT="2025-05-08T15:38:14.08Z" personId="{13C37F2E-4D51-E3EE-FC14-919C7A23FB02}" id="{A12F5487-BD0A-1D55-ECB3-5B2E3E52411C}" done="0">
+  <threadedComment ref="G51" dT="2025-05-08T15:38:14.08Z" personId="{97EA6DEE-8592-7F06-E67E-CB747DF27A81}" id="{A12F5487-BD0A-1D55-ECB3-5B2E3E52411C}" done="0">
     <text xml:space="preserve">é necessari conhecimento sobre a api de reatividade do java, para entender os conceitos avançados de r2dbc
 </text>
   </threadedComment>
@@ -23826,19 +23826,23 @@
       <c r="K26" s="4"/>
     </row>
     <row r="27" ht="38.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="7">
         <v>4</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4">
+      <c r="C27" s="7"/>
+      <c r="D27" s="7">
         <v>4</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="E27" s="7">
+        <v>5</v>
+      </c>
+      <c r="F27" s="7">
+        <v>1</v>
+      </c>
+      <c r="G27" s="7"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -48903,7 +48907,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{000C006A-00D4-4D26-BB3C-0065003700AE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00A70078-005A-4048-902B-003A00B70002}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
           <x14:formula1>
             <xm:f>"Feeling sobre o quão confortável está com aquilo,Usa a llm pedindo feedback (óbvio que a llm pode errar),Comparação do que você fez com de outra pessoa com um nível de senioridade maior,Postagem do que você fez em redes públicas para tentar pegar feedback"&amp;".  ,Feedbacks de pares do trabalho sobre determinado fase do plano, entregável, entendimento etc,Acesso a uma pessoa professora que pode te dar feedback direto"</xm:f>
           </x14:formula1>

</xml_diff>